<commit_message>
Add extension markup menu for genre and rework enum
</commit_message>
<xml_diff>
--- a/TelegramBot/base.xlsx
+++ b/TelegramBot/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myros\source\repos\TelegramBot\TelegramBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB728DD-CCF0-4E6A-8DAF-B1A8077550B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FADA803-026A-4C10-B951-EE12F287C4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2490" windowWidth="28425" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Для чого ти потрібен?</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Текст</t>
   </si>
   <si>
-    <t>Історичне</t>
-  </si>
-  <si>
     <t>https://uakino.club/uploads/mini/serial/fe/0d580dd118f183f48a95136d10b82c.jpg</t>
   </si>
   <si>
@@ -89,6 +86,33 @@
   </si>
   <si>
     <t>Jonh Week</t>
+  </si>
+  <si>
+    <t>Комедія</t>
+  </si>
+  <si>
+    <t>Документальний фільм</t>
+  </si>
+  <si>
+    <t>Містика</t>
+  </si>
+  <si>
+    <t>Фантастика</t>
+  </si>
+  <si>
+    <t>Історична драма</t>
+  </si>
+  <si>
+    <t>Анімація</t>
+  </si>
+  <si>
+    <t>Екшн</t>
+  </si>
+  <si>
+    <t>Трилер</t>
+  </si>
+  <si>
+    <t>Романтика</t>
   </si>
 </sst>
 </file>
@@ -464,14 +488,14 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
   </cols>
@@ -484,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1">
         <v>5</v>
@@ -493,18 +517,18 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>4.55</v>
@@ -513,18 +537,18 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1">
         <v>3.78</v>
@@ -533,18 +557,18 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>3.8</v>
@@ -553,18 +577,18 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>4.9000000000000004</v>
@@ -573,18 +597,18 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1">
         <v>4.0999999999999996</v>
@@ -593,18 +617,18 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1">
         <v>4.2</v>
@@ -613,18 +637,18 @@
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -633,18 +657,18 @@
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>2.85</v>
@@ -653,18 +677,18 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1">
         <v>4.5</v>
@@ -673,7 +697,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>